<commit_message>
Probability, exclusive events, and independent events
</commit_message>
<xml_diff>
--- a/Homework/JulyExclusiveandIndependentHW.xlsx
+++ b/Homework/JulyExclusiveandIndependentHW.xlsx
@@ -1,30 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\edxtake2module1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anguyen\Documents\GitHub\Stats using Excel\stats-primer\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EF45D8-FEF7-4782-B1E2-7B0B9BC276D2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Homework 2_3</t>
   </si>
@@ -72,12 +78,33 @@
   </si>
   <si>
     <t>3..Suppose we randomly choose an integer between</t>
+  </si>
+  <si>
+    <t>2 dices, at least one 4</t>
+  </si>
+  <si>
+    <t>2-6,3-5,4-4,5-3,6-2</t>
+  </si>
+  <si>
+    <t>2,3,5,7</t>
+  </si>
+  <si>
+    <t>p(a)</t>
+  </si>
+  <si>
+    <t>p(b)</t>
+  </si>
+  <si>
+    <t>p(a and b)</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,10 +148,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="13" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,19 +434,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -424,91 +454,138 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="J5" s="5">
+        <f>11/36</f>
+        <v>0.30555555555555558</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="L9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="J10" s="1">
+        <f>1/9+1/8+1/17</f>
+        <v>0.29493464052287582</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="J17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="1" t="str">
+        <f>"4/10"</f>
+        <v>4/10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="J18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="4" t="str">
+        <f>"5/10"</f>
+        <v>5/10</v>
+      </c>
+      <c r="M18" s="1" t="str">
+        <f>"20/100 or 2/10"</f>
+        <v>20/100 or 2/10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="K20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="4" t="str">
+        <f>"3/10"</f>
+        <v>3/10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>